<commit_message>
fix: Improve file upload handling and robustness
Enhance robustness and flexibility of data import, improving user experience and fix CSV import bug to properly handle files with different delimiters.
- Handle CSV, XLSX, ODS, and XLS file uploads with various delimiters.
- Automatically detect delimiters in CSV files, including comma, semicolon, and tab.
- Support tables with and without headers during file upload.
- Ignore rows containing non-numeric values or invalid data (e.g., strings or NA).
- Ensure invalid rows are removed to prevent errors during data processing.
</commit_message>
<xml_diff>
--- a/data/raw/sample_data.xlsx
+++ b/data/raw/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sync\03_projects\data_science\projects\easycalibrate\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3850CE6-FA5B-405A-BA16-CFF80FBC4241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92335B92-86F5-4647-8BBB-8F400047D6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,16 +46,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,11 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -374,7 +363,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -383,202 +372,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>0.05</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>9.1027749999999994</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>0.05</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>9.1029710000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>0.05</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>9.0967319999999994</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>0.125</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>22.658197999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>0.125</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>22.882701000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>0.125</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>22.830106000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>0.5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>77.690938000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>0.5</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>75.064286999999993</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>0.5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>80.320071999999996</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>1.25</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>197.03014899999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>1.25</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>197.390646</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>1.25</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>196.477779</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>2.5</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>388.543543</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>2.5</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>382.67299200000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>2.5</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>378.27337199999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>844.93752099999995</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>5</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>799.80493200000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>5</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>799.69575199999997</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>12.5</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1996.3672240000001</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>12.5</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1987.8437019999999</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>12.5</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1969.8420719999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>25</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>3901.9778799999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>25</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>3786.6928670000002</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>25</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>3762.2910019999999</v>
       </c>
     </row>

</xml_diff>